<commit_message>
ITMO unique identifiers as per 6/CMA.4 annex I para 3.  Allow '+' character in for activity type names
</commit_message>
<xml_diff>
--- a/AEF_files/Guyana 2022 correct.syntax_checked.xlsx
+++ b/AEF_files/Guyana 2022 correct.syntax_checked.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="9940" yWindow="2200" windowWidth="39680" windowHeight="19760" tabRatio="618" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="9940" yWindow="2200" windowWidth="39680" windowHeight="19760" tabRatio="618" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" state="visible" r:id="rId1"/>
@@ -34,7 +34,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -195,6 +195,12 @@
       <family val="1"/>
       <color theme="1"/>
       <sz val="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -591,6 +597,12 @@
     <xf numFmtId="164" fontId="18" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="23" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -611,20 +623,14 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -758,6 +764,11 @@
         <t>All field content valid.</t>
       </text>
     </comment>
+    <comment ref="I9" authorId="0" shapeId="0">
+      <text>
+        <t>Cell content error: The value provided for 'First ID' must be an ITMO unique identifier as per 6/CMA.4 annex I para.3.</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -771,6 +782,11 @@
     <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <t>All field content valid.</t>
+      </text>
+    </comment>
+    <comment ref="F8" authorId="0" shapeId="0">
+      <text>
+        <t>Cell content error: The value provided for 'First ID' must be an ITMO unique identifier as per 6/CMA.4 annex I para.3.</t>
       </text>
     </comment>
   </commentList>
@@ -2426,7 +2442,7 @@
       </c>
     </row>
     <row r="13" ht="16" customHeight="1" thickTop="1">
-      <c r="B13" s="92" t="n"/>
+      <c r="B13" s="94" t="n"/>
       <c r="C13" s="101" t="n"/>
     </row>
   </sheetData>
@@ -2448,7 +2464,7 @@
   <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2490,7 +2506,7 @@
       </c>
     </row>
     <row r="5" ht="14.5" customHeight="1">
-      <c r="B5" s="93" t="inlineStr">
+      <c r="B5" s="95" t="inlineStr">
         <is>
           <t>Authorization</t>
         </is>
@@ -2682,7 +2698,7 @@
       </c>
       <c r="L8" s="85" t="inlineStr">
         <is>
-          <t>REDD</t>
+          <t>REDD+</t>
         </is>
       </c>
       <c r="M8" s="86" t="inlineStr">
@@ -2703,7 +2719,7 @@
       </c>
       <c r="Q8" s="19" t="inlineStr">
         <is>
-          <t>2030 - 2035</t>
+          <t>Use: from 2030 to 2035</t>
         </is>
       </c>
       <c r="R8" s="19" t="n"/>
@@ -2866,8 +2882,8 @@
   </sheetPr>
   <dimension ref="A1:AH13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y9" sqref="Y9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3047,14 +3063,14 @@
       <c r="V6" s="38" t="n"/>
       <c r="W6" s="38" t="n"/>
       <c r="X6" s="36" t="n"/>
-      <c r="Y6" s="95" t="inlineStr">
+      <c r="Y6" s="97" t="inlineStr">
         <is>
           <t xml:space="preserve"> Transfer / Acquisition</t>
         </is>
       </c>
       <c r="Z6" s="102" t="n"/>
       <c r="AA6" s="40" t="n"/>
-      <c r="AB6" s="94" t="inlineStr">
+      <c r="AB6" s="96" t="inlineStr">
         <is>
           <t>Use or cancellation</t>
         </is>
@@ -3252,8 +3268,8 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="56" customHeight="1">
-      <c r="B9" s="99" t="n">
+    <row r="9" ht="70" customHeight="1">
+      <c r="B9" s="92" t="n">
         <v>45292</v>
       </c>
       <c r="C9" s="24" t="inlineStr">
@@ -3288,12 +3304,12 @@
       </c>
       <c r="I9" s="87" t="inlineStr">
         <is>
-          <t>CA0005-ART-GY-1-2022</t>
+          <t>CA0005-GUY01-GUY-1-2022</t>
         </is>
       </c>
       <c r="J9" s="88" t="inlineStr">
         <is>
-          <t>CA0005-ART-GY-8,732,929-2022</t>
+          <t>CA0005-GUY01-GUY-8,732,929-2022</t>
         </is>
       </c>
       <c r="K9" s="19" t="n"/>
@@ -3505,7 +3521,7 @@
   <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F8" sqref="F8:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3537,7 +3553,7 @@
     </row>
     <row r="2"/>
     <row r="3" ht="16" customHeight="1" thickBot="1">
-      <c r="B3" s="97" t="inlineStr">
+      <c r="B3" s="99" t="inlineStr">
         <is>
           <t>Table 4: Holdings</t>
         </is>
@@ -3552,7 +3568,7 @@
       <c r="J3" s="103" t="n"/>
       <c r="K3" s="103" t="n"/>
       <c r="L3" s="50" t="n"/>
-      <c r="M3" s="98" t="n"/>
+      <c r="M3" s="100" t="n"/>
       <c r="N3" s="103" t="n"/>
       <c r="O3" s="103" t="n"/>
       <c r="P3" s="103" t="n"/>
@@ -3566,7 +3582,7 @@
       <c r="C4" s="67" t="n"/>
       <c r="D4" s="68" t="n"/>
       <c r="E4" s="67" t="n"/>
-      <c r="F4" s="96" t="inlineStr">
+      <c r="F4" s="98" t="inlineStr">
         <is>
           <t>Unique identifiers</t>
         </is>
@@ -3577,7 +3593,7 @@
       <c r="J4" s="104" t="n"/>
       <c r="K4" s="104" t="n"/>
       <c r="L4" s="69" t="n"/>
-      <c r="M4" s="96" t="inlineStr">
+      <c r="M4" s="98" t="inlineStr">
         <is>
           <t>Metric and quantity</t>
         </is>
@@ -3587,7 +3603,7 @@
       <c r="P4" s="104" t="n"/>
       <c r="Q4" s="104" t="n"/>
       <c r="R4" s="69" t="n"/>
-      <c r="S4" s="96" t="inlineStr">
+      <c r="S4" s="98" t="inlineStr">
         <is>
           <t>ITMO details</t>
         </is>
@@ -3600,14 +3616,14 @@
       <c r="C5" s="23" t="n"/>
       <c r="D5" s="38" t="n"/>
       <c r="E5" s="38" t="n"/>
-      <c r="F5" s="94" t="inlineStr">
+      <c r="F5" s="96" t="inlineStr">
         <is>
           <t>ITMO unique identifier</t>
         </is>
       </c>
       <c r="G5" s="102" t="n"/>
       <c r="H5" s="18" t="n"/>
-      <c r="I5" s="94" t="inlineStr">
+      <c r="I5" s="96" t="inlineStr">
         <is>
           <t>Underlying units</t>
         </is>
@@ -3634,7 +3650,7 @@
       <c r="G6" s="37" t="n"/>
       <c r="H6" s="18" t="n"/>
       <c r="I6" s="23" t="n"/>
-      <c r="J6" s="94" t="inlineStr">
+      <c r="J6" s="96" t="inlineStr">
         <is>
           <t>Underlying unit unique identifier</t>
         </is>
@@ -3737,7 +3753,7 @@
       </c>
       <c r="U7" s="21" t="n"/>
     </row>
-    <row r="8" ht="56" customHeight="1">
+    <row r="8" ht="70" customHeight="1">
       <c r="B8" s="82" t="inlineStr">
         <is>
           <t>CA0005</t>
@@ -3760,12 +3776,12 @@
       </c>
       <c r="F8" s="87" t="inlineStr">
         <is>
-          <t>CA0005-ART-GY-1-2022</t>
+          <t>CA0005-GUY01-GUY-1-2022</t>
         </is>
       </c>
       <c r="G8" s="88" t="inlineStr">
         <is>
-          <t>CA0005-ART-GY-8,732,929-2022</t>
+          <t>CA0005-GUY01-GUY-8,732,929-2022</t>
         </is>
       </c>
       <c r="H8" s="19" t="n"/>
@@ -4252,7 +4268,7 @@
   </sheetPr>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -4287,7 +4303,7 @@
     </row>
     <row r="9" ht="15" customHeight="1">
       <c r="C9" s="51" t="n"/>
-      <c r="D9" s="94" t="inlineStr">
+      <c r="D9" s="96" t="inlineStr">
         <is>
           <t>Authorized entity</t>
         </is>
@@ -4344,7 +4360,7 @@
       <c r="K10" s="53" t="n"/>
     </row>
     <row r="11">
-      <c r="C11" s="100" t="n">
+      <c r="C11" s="93" t="n">
         <v>45707</v>
       </c>
       <c r="D11" s="53" t="n"/>
@@ -4725,8 +4741,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008FB6730B0802B54A9F00C78B857E1443" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3aa8ea1b9f2e27c2fdef6ef4056186e5">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="819ae873-75e1-413b-9d00-7af9258cf281" xmlns:ns3="eb4559c4-8463-4985-927f-f0d558bff8f0" xmlns:ns4="13d80b15-5f07-43ab-b435-85767a7dac08" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="16259e29b70fac56f05f7b64cc1f875d" ns2:_="" ns3:_="" ns4:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008FB6730B0802B54A9F00C78B857E1443" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e7d0671dbe340d15fdce5ab7e9f4c491">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="819ae873-75e1-413b-9d00-7af9258cf281" xmlns:ns3="eb4559c4-8463-4985-927f-f0d558bff8f0" xmlns:ns4="13d80b15-5f07-43ab-b435-85767a7dac08" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2feafd61044eb4abe44eb47c2e62f3e5" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="819ae873-75e1-413b-9d00-7af9258cf281"/>
     <xsd:import namespace="eb4559c4-8463-4985-927f-f0d558bff8f0"/>
     <xsd:import namespace="13d80b15-5f07-43ab-b435-85767a7dac08"/>
@@ -5036,17 +5052,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70B99BA5-63C4-47F8-A3C5-CE0F09C159FE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E66A704-18A3-4F94-977E-5AB254D0AA02}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C5A3556-201D-4E76-AFC8-DC48DE99841F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DE0840C-BC11-4BC1-A7C8-55D99CE03D98}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3724E610-97EC-41C8-8530-0EE0CFD71C48}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6E58CCB-ABA3-4E5E-9953-224F70B152BB}"/>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C96F96E3-1A05-4D49-807B-AB66CECA8346}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F221066-6B9C-4D90-AC82-56FEB309767F}"/>
 </file>
</xml_diff>